<commit_message>
Latest Change August 2023 - PowerSupply
</commit_message>
<xml_diff>
--- a/NodeRed/Rotator Direction Scaling.xlsx
+++ b/NodeRed/Rotator Direction Scaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b2e3be082d3b3d0/Documents/Amateur Radio/RemoteHF/RemoteHF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b2e3be082d3b3d0/Documents/Amateur Radio/RemoteHF/NodeRed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{151B0727-B25B-44EF-82B1-87033397B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF4FD436-2501-4553-B1E8-2C950F605DDF}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{151B0727-B25B-44EF-82B1-87033397B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2688345-C4F9-4BB5-AC37-2ABAC693FE0D}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="990" windowWidth="16665" windowHeight="19575" xr2:uid="{1446005F-4E49-435B-81AE-6B414259F8A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" xr2:uid="{1446005F-4E49-435B-81AE-6B414259F8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Volts</t>
   </si>
   <si>
     <t>Degrees</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
@@ -94,6 +109,59 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>608914</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>180833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D31A51E6-0869-035C-DFF9-2389022EC2ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="8382000"/>
+          <a:ext cx="5485714" cy="1133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CC4833-5D27-43FA-B672-059999E22FDF}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +736,45 @@
         <v>450</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2.0979999999999999</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Node Red JSON
</commit_message>
<xml_diff>
--- a/NodeRed/Rotator Direction Scaling.xlsx
+++ b/NodeRed/Rotator Direction Scaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b2e3be082d3b3d0/Documents/Amateur Radio/RemoteHF/NodeRed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{151B0727-B25B-44EF-82B1-87033397B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2688345-C4F9-4BB5-AC37-2ABAC693FE0D}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{151B0727-B25B-44EF-82B1-87033397B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32D3F4F1-1906-40F6-8BC9-B82EFC946711}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" xr2:uid="{1446005F-4E49-435B-81AE-6B414259F8A3}"/>
+    <workbookView xWindow="19200" yWindow="795" windowWidth="20670" windowHeight="19575" xr2:uid="{1446005F-4E49-435B-81AE-6B414259F8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Volts</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Min</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>Millivolts</t>
   </si>
 </sst>
 </file>
@@ -158,10 +164,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -461,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CC4833-5D27-43FA-B672-059999E22FDF}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,39 +738,91 @@
         <v>450</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1.41</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>200</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.82499999999999996</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>800</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.20399999999999999</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>1400</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2.0979999999999999</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>2000</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>2600</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>6</v>
       </c>

</xml_diff>